<commit_message>
add tutorial and more info on readme.md
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="student_info" sheetId="1" r:id="rId1"/>
+    <sheet name="Ví dụ" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>student_name</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Phan Quốc Hưng</t>
+  </si>
+  <si>
+    <t>Một số lỗi thường gặp</t>
+  </si>
+  <si>
+    <t>- Tên hình ảnh sản phẩm không giống với tên file hình trong thư mục, hoặc quên ghi đuôi .png/.jpg/.jpeg</t>
+  </si>
+  <si>
+    <t>- Tên khóa học ký tự viết hoa chưa giống</t>
   </si>
 </sst>
 </file>
@@ -107,13 +117,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -397,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,4 +502,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>84972235270</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>84937285555</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
release v0.0.2, fixing minor things in printing
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="student_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>student_name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Bé làm Game</t>
   </si>
   <si>
-    <t>test.png</t>
-  </si>
-  <si>
     <t>Phan Quốc Hưng</t>
   </si>
   <si>
@@ -65,6 +62,12 @@
   </si>
   <si>
     <t>- Tên khóa học ký tự viết hoa chưa giống</t>
+  </si>
+  <si>
+    <t>quochung.jpg</t>
+  </si>
+  <si>
+    <t>vyan.jpg</t>
   </si>
 </sst>
 </file>
@@ -415,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,13 +470,13 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>84937285555</v>
@@ -490,8 +493,8 @@
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -508,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,12 +563,12 @@
         <v>4</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>84937285555</v>
@@ -583,22 +586,22 @@
         <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>